<commit_message>
Backup before major refactoring
</commit_message>
<xml_diff>
--- a/BoxTask/ID_21.xlsx
+++ b/BoxTask/ID_21.xlsx
@@ -8,13 +8,21 @@
   </bookViews>
   <sheets>
     <sheet name="block1_trial1" sheetId="1" r:id="rId1"/>
+    <sheet name="block1_trial2" sheetId="2" r:id="rId2"/>
+    <sheet name="block1_trial3" sheetId="3" r:id="rId3"/>
+    <sheet name="block2_trial1" sheetId="4" r:id="rId4"/>
+    <sheet name="block2_trial2" sheetId="5" r:id="rId5"/>
+    <sheet name="block2_trial3" sheetId="6" r:id="rId6"/>
+    <sheet name="block3_trial1" sheetId="7" r:id="rId7"/>
+    <sheet name="block3_trial2" sheetId="8" r:id="rId8"/>
+    <sheet name="block3_trial3" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
   <si>
     <t>Box_Num</t>
   </si>
@@ -29,6 +37,30 @@
   </si>
   <si>
     <t>#0000FF</t>
+  </si>
+  <si>
+    <t>#FFD700</t>
+  </si>
+  <si>
+    <t>#800080</t>
+  </si>
+  <si>
+    <t>#00BFFF</t>
+  </si>
+  <si>
+    <t>#FFFF00</t>
+  </si>
+  <si>
+    <t>#BA55D3</t>
+  </si>
+  <si>
+    <t>#FF4500</t>
+  </si>
+  <si>
+    <t>#FF69B4</t>
+  </si>
+  <si>
+    <t>#87CEFA</t>
   </si>
 </sst>
 </file>
@@ -386,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,13 +446,688 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>1.637437399986084</v>
+        <v>0.9887788999985787</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1.19843970000511</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0.6700587999948766</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.8839977000025101</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>0.8153476000006776</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>0.8358997999966959</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.843316300000879</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0.7260068000032334</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0.787659599998733</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0.7117578999968828</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0.7910781999962637</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1.086166100001719</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0.8779292000035639</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0.9268933999992441</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>1.184310299999197</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.8738451999961399</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0.818136299996695</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.8501193999982206</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0.8575541999962297</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0.6914394999985234</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0.9617148000033922</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0.7800151999981608</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0.8502520000038203</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.7838176000004751</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0.7237789999999222</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>0.6622744999986026</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1.058566599996993</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0.6220011999976123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Graphics and summary output reworked
Graphical flow and design is complete. Need to find a way to append to the summary excel file.
</commit_message>
<xml_diff>
--- a/BoxTask/ID_21.xlsx
+++ b/BoxTask/ID_21.xlsx
@@ -7,16 +7,45 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="block0_trial1" sheetId="1" r:id="rId1"/>
+    <sheet name="block1_trial2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+  <si>
+    <t>Box_Num</t>
+  </si>
+  <si>
+    <t>Probability_Estimates</t>
+  </si>
+  <si>
+    <t>Reaction_time</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>#0000FF</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +61,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +69,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +387,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.8227142999967327</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0.8621263999993971</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.7671456999996735</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0.6203459999996994</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1.287835400002223</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1.044512500000565</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0.5653464999995776</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0.8708101999982318</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Summary output is reworked
Summary output is reworked. Need to make it so that all ratings are numbers and that text and code is clean
</commit_message>
<xml_diff>
--- a/BoxTask/ID_21.xlsx
+++ b/BoxTask/ID_21.xlsx
@@ -9,13 +9,24 @@
   <sheets>
     <sheet name="block0_trial1" sheetId="1" r:id="rId1"/>
     <sheet name="block1_trial2" sheetId="2" r:id="rId2"/>
+    <sheet name="block1_trial3" sheetId="3" r:id="rId3"/>
+    <sheet name="block1_trial4" sheetId="4" r:id="rId4"/>
+    <sheet name="1_answered" sheetId="5" r:id="rId5"/>
+    <sheet name="block2_trial5" sheetId="6" r:id="rId6"/>
+    <sheet name="block2_trial6" sheetId="7" r:id="rId7"/>
+    <sheet name="block2_trial7" sheetId="8" r:id="rId8"/>
+    <sheet name="2_answered" sheetId="9" r:id="rId9"/>
+    <sheet name="block3_trial8" sheetId="10" r:id="rId10"/>
+    <sheet name="block3_trial9" sheetId="11" r:id="rId11"/>
+    <sheet name="block3_trial10" sheetId="12" r:id="rId12"/>
+    <sheet name="3_answered" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
   <si>
     <t>Box_Num</t>
   </si>
@@ -30,6 +41,33 @@
   </si>
   <si>
     <t>#0000FF</t>
+  </si>
+  <si>
+    <t>#FFD700</t>
+  </si>
+  <si>
+    <t>#800080</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>#00BFFF</t>
+  </si>
+  <si>
+    <t>#FFFF00</t>
+  </si>
+  <si>
+    <t>#BA55D3</t>
+  </si>
+  <si>
+    <t>#FF4500</t>
+  </si>
+  <si>
+    <t>#FF69B4</t>
+  </si>
+  <si>
+    <t>#87CEFA</t>
   </si>
 </sst>
 </file>
@@ -387,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,7 +456,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0.8227142999967327</v>
+        <v>0.6755552999966312</v>
       </c>
       <c r="E2">
         <v>-1</v>
@@ -432,23 +470,40 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>0.8621263999993971</v>
-      </c>
-      <c r="E3" t="s">
+        <v>0.7322296999991522</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>4</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+      <c r="D4">
+        <v>0.5289755999983754</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,95 +534,416 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0.7671456999996735</v>
-      </c>
-      <c r="E2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
+        <v>0.6272623999975622</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.5794945999950869</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>0.6203459999996994</v>
-      </c>
-      <c r="E3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
+      <c r="D2">
+        <v>1.132582800004457</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>1.287835400002223</v>
-      </c>
-      <c r="E4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
+      <c r="D2">
+        <v>0.5229143999968073</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0.5489873999977135</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0.557427200001257</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1.044512500000565</v>
-      </c>
-      <c r="E5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
+      <c r="D2">
+        <v>0.6468434999987949</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0.5490627000035602</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>0.5653464999995776</v>
-      </c>
-      <c r="E6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>0.8708101999982318</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
+      <c r="D2">
+        <v>0.9740508999966551</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>